<commit_message>
Tidied up spreadsheet from spring 2019
</commit_message>
<xml_diff>
--- a/StudentGuideModule2/what_labs_to_include/132 lab list for 2019 spring.xlsx
+++ b/StudentGuideModule2/what_labs_to_include/132 lab list for 2019 spring.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mtrawick\Desktop\github\132\StudentGuideModule2\what_labs_to_include\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="18780" yWindow="5140" windowWidth="26620" windowHeight="15940" tabRatio="541"/>
+    <workbookView xWindow="18780" yWindow="5136" windowWidth="26616" windowHeight="15936" tabRatio="541"/>
   </bookViews>
   <sheets>
     <sheet name="lablist" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="330"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="330"/>
     </ext>
   </extLst>
 </workbook>
@@ -28,7 +33,7 @@
     <author>Matt Trawick</author>
   </authors>
   <commentList>
-    <comment ref="C1" authorId="0">
+    <comment ref="C1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -54,7 +59,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0">
+    <comment ref="F1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -78,7 +83,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X1" authorId="0">
+    <comment ref="X1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -105,7 +110,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M7" authorId="0">
+    <comment ref="M7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -125,12 +130,13 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-This lab is definitely on a tangential topic, but it is fun and only takes about 15 minutes.  That said, I can totally understand why others might not want to do this lab.
-</t>
+This lab is definitely on a tangential topic, but it is fun and only takes about 15 minutes.  
+I also personally like it because I'm a former musician, and this makes a nice connection with some of my students.  
+That said, I can totally understand why others might not want to do this lab.</t>
         </r>
       </text>
     </comment>
-    <comment ref="M8" authorId="0">
+    <comment ref="M8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -156,7 +162,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M10" authorId="0">
+    <comment ref="M10" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -182,7 +188,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y11" authorId="0">
+    <comment ref="Y11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -207,7 +213,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K12" authorId="0">
+    <comment ref="K12" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -231,7 +237,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M19" authorId="0">
+    <comment ref="M19" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -257,7 +263,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z19" authorId="0">
+    <comment ref="Z19" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -282,7 +288,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y21" authorId="0">
+    <comment ref="Y21" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -306,7 +312,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M22" authorId="0">
+    <comment ref="M22" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -333,7 +339,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M23" authorId="0">
+    <comment ref="M23" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -357,7 +363,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K25" authorId="0">
+    <comment ref="K25" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -381,7 +387,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M25" authorId="0">
+    <comment ref="M25" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -406,7 +412,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O25" authorId="0">
+    <comment ref="O25" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -421,7 +427,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X25" authorId="0">
+    <comment ref="X25" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -445,7 +451,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y25" authorId="0">
+    <comment ref="Y25" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -469,7 +475,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA25" authorId="0">
+    <comment ref="AA25" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -494,7 +500,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O26" authorId="0">
+    <comment ref="O26" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -509,7 +515,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M28" authorId="0">
+    <comment ref="M28" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -533,7 +539,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K29" authorId="0">
+    <comment ref="K29" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -558,7 +564,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M29" authorId="0">
+    <comment ref="M29" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -582,7 +588,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K30" authorId="0">
+    <comment ref="K30" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -607,7 +613,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M30" authorId="0">
+    <comment ref="M30" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -631,7 +637,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M33" authorId="0">
+    <comment ref="M33" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -656,7 +662,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M36" authorId="0">
+    <comment ref="M36" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -680,7 +686,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M41" authorId="0">
+    <comment ref="M41" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -705,7 +711,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M42" authorId="0">
+    <comment ref="M42" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -731,7 +737,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M48" authorId="0">
+    <comment ref="M48" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -755,7 +761,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M49" authorId="0">
+    <comment ref="M49" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -780,7 +786,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M51" authorId="0">
+    <comment ref="M51" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -804,7 +810,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M54" authorId="0">
+    <comment ref="M54" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -829,7 +835,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M57" authorId="0">
+    <comment ref="M57" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -853,7 +859,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M60" authorId="0">
+    <comment ref="M60" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -878,7 +884,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M67" authorId="0">
+    <comment ref="M67" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1586,7 +1592,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -2212,7 +2218,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2423,6 +2429,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -2846,32 +2855,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S28" sqref="S28"/>
+      <selection pane="bottomLeft" activeCell="K70" sqref="K70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.83203125" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.83203125" style="23" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.77734375" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.77734375" style="23" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.33203125" style="23" customWidth="1"/>
-    <col min="4" max="4" width="8.1640625" style="14" customWidth="1"/>
-    <col min="5" max="10" width="5.83203125" style="14" customWidth="1"/>
-    <col min="11" max="11" width="28.5" style="20" customWidth="1"/>
-    <col min="12" max="12" width="8.83203125" style="2" customWidth="1"/>
-    <col min="13" max="13" width="8.83203125" style="20" customWidth="1"/>
-    <col min="14" max="15" width="8.83203125" style="2" customWidth="1"/>
-    <col min="16" max="16" width="8.83203125" style="34" customWidth="1"/>
-    <col min="17" max="21" width="8.83203125" style="83" customWidth="1"/>
+    <col min="4" max="4" width="8.109375" style="14" customWidth="1"/>
+    <col min="5" max="10" width="5.77734375" style="14" customWidth="1"/>
+    <col min="11" max="11" width="28.44140625" style="20" customWidth="1"/>
+    <col min="12" max="12" width="8.77734375" style="2" customWidth="1"/>
+    <col min="13" max="13" width="8.77734375" style="20" customWidth="1"/>
+    <col min="14" max="15" width="8.77734375" style="2" customWidth="1"/>
+    <col min="16" max="16" width="8.77734375" style="34" customWidth="1"/>
+    <col min="17" max="21" width="8.77734375" style="83" customWidth="1"/>
     <col min="22" max="22" width="11" style="3" customWidth="1"/>
-    <col min="23" max="23" width="2.5" style="3" customWidth="1"/>
+    <col min="23" max="23" width="2.44140625" style="3" customWidth="1"/>
     <col min="24" max="24" width="10.33203125" style="3" customWidth="1"/>
-    <col min="26" max="26" width="9.5" customWidth="1"/>
-    <col min="27" max="27" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.44140625" customWidth="1"/>
+    <col min="27" max="27" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" s="1" customFormat="1" ht="42">
+    <row r="1" spans="1:31" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="48" t="s">
         <v>76</v>
       </c>
@@ -2948,7 +2957,7 @@
       <c r="AD1" s="33"/>
       <c r="AE1" s="33"/>
     </row>
-    <row r="2" spans="1:31" s="1" customFormat="1">
+    <row r="2" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>104</v>
       </c>
@@ -3011,7 +3020,7 @@
       <c r="AD2" s="33"/>
       <c r="AE2" s="33"/>
     </row>
-    <row r="3" spans="1:31" s="1" customFormat="1">
+    <row r="3" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="48"/>
       <c r="B3" s="54" t="s">
         <v>106</v>
@@ -3058,7 +3067,7 @@
         <v>1</v>
       </c>
       <c r="U3" s="88"/>
-      <c r="V3" s="75">
+      <c r="V3" s="89">
         <f t="shared" ref="V3:V66" si="1">SUM(R3:U3)</f>
         <v>2</v>
       </c>
@@ -3072,7 +3081,7 @@
       <c r="AD3" s="33"/>
       <c r="AE3" s="33"/>
     </row>
-    <row r="4" spans="1:31" s="1" customFormat="1">
+    <row r="4" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="30" t="s">
         <v>73</v>
       </c>
@@ -3149,7 +3158,7 @@
       <c r="AD4" s="33"/>
       <c r="AE4" s="33"/>
     </row>
-    <row r="5" spans="1:31">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B5" s="23" t="s">
         <v>158</v>
       </c>
@@ -3220,7 +3229,7 @@
       <c r="AD5" s="33"/>
       <c r="AE5" s="33"/>
     </row>
-    <row r="6" spans="1:31">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A6" s="30"/>
       <c r="B6" s="31" t="s">
         <v>159</v>
@@ -3281,7 +3290,7 @@
       <c r="AD6" s="33"/>
       <c r="AE6" s="33"/>
     </row>
-    <row r="7" spans="1:31" s="33" customFormat="1">
+    <row r="7" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="48"/>
       <c r="B7" s="24" t="s">
         <v>183</v>
@@ -3320,7 +3329,7 @@
       <c r="S7" s="86"/>
       <c r="T7" s="86"/>
       <c r="U7" s="86"/>
-      <c r="V7" s="75">
+      <c r="V7" s="89">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3329,7 +3338,7 @@
       <c r="Z7" s="5"/>
       <c r="AA7" s="15"/>
     </row>
-    <row r="8" spans="1:31">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A8" s="30" t="s">
         <v>74</v>
       </c>
@@ -3397,7 +3406,7 @@
       <c r="AD8" s="33"/>
       <c r="AE8" s="33"/>
     </row>
-    <row r="9" spans="1:31">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B9" s="23" t="s">
         <v>113</v>
       </c>
@@ -3461,7 +3470,7 @@
       <c r="AD9" s="33"/>
       <c r="AE9" s="33"/>
     </row>
-    <row r="10" spans="1:31" ht="15" thickBot="1">
+    <row r="10" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="23" t="s">
         <v>114</v>
       </c>
@@ -3516,7 +3525,7 @@
       <c r="AD10" s="33"/>
       <c r="AE10" s="33"/>
     </row>
-    <row r="11" spans="1:31">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B11" s="23" t="s">
         <v>115</v>
       </c>
@@ -3582,7 +3591,7 @@
       <c r="AD11" s="33"/>
       <c r="AE11" s="33"/>
     </row>
-    <row r="12" spans="1:31" ht="15" thickBot="1">
+    <row r="12" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="23" t="s">
         <v>185</v>
       </c>
@@ -3643,7 +3652,7 @@
       <c r="AD12" s="33"/>
       <c r="AE12" s="33"/>
     </row>
-    <row r="13" spans="1:31">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B13" s="23" t="s">
         <v>188</v>
       </c>
@@ -3717,7 +3726,7 @@
       <c r="AD13" s="33"/>
       <c r="AE13" s="33"/>
     </row>
-    <row r="14" spans="1:31" ht="15" thickBot="1">
+    <row r="14" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="23" t="s">
         <v>186</v>
       </c>
@@ -3780,7 +3789,7 @@
       <c r="AD14" s="33"/>
       <c r="AE14" s="33"/>
     </row>
-    <row r="15" spans="1:31">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B15" s="23" t="s">
         <v>187</v>
       </c>
@@ -3843,7 +3852,7 @@
       <c r="AD15" s="33"/>
       <c r="AE15" s="33"/>
     </row>
-    <row r="16" spans="1:31">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B16" s="23" t="s">
         <v>116</v>
       </c>
@@ -3914,7 +3923,7 @@
       <c r="AD16" s="33"/>
       <c r="AE16" s="33"/>
     </row>
-    <row r="17" spans="1:31">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B17" s="23" t="s">
         <v>117</v>
       </c>
@@ -3958,7 +3967,7 @@
       <c r="AD17" s="33"/>
       <c r="AE17" s="33"/>
     </row>
-    <row r="18" spans="1:31">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B18" s="23" t="s">
         <v>118</v>
       </c>
@@ -4007,7 +4016,7 @@
       <c r="AD18" s="33"/>
       <c r="AE18" s="33"/>
     </row>
-    <row r="19" spans="1:31" ht="15" thickBot="1">
+    <row r="19" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="23" t="s">
         <v>119</v>
       </c>
@@ -4050,7 +4059,7 @@
       <c r="U19" s="83">
         <v>1</v>
       </c>
-      <c r="V19" s="75">
+      <c r="V19" s="89">
         <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
@@ -4068,7 +4077,7 @@
       <c r="AD19" s="33"/>
       <c r="AE19" s="33"/>
     </row>
-    <row r="20" spans="1:31" ht="15" thickBot="1">
+    <row r="20" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="11" t="s">
         <v>75</v>
       </c>
@@ -4136,7 +4145,7 @@
       <c r="AD20" s="33"/>
       <c r="AE20" s="33"/>
     </row>
-    <row r="21" spans="1:31">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B21" s="23" t="s">
         <v>121</v>
       </c>
@@ -4211,7 +4220,7 @@
       <c r="AD21" s="33"/>
       <c r="AE21" s="33"/>
     </row>
-    <row r="22" spans="1:31" ht="15" thickBot="1">
+    <row r="22" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="23" t="s">
         <v>204</v>
       </c>
@@ -4259,7 +4268,7 @@
       <c r="AD22" s="33"/>
       <c r="AE22" s="33"/>
     </row>
-    <row r="23" spans="1:31">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B23" s="23" t="s">
         <v>122</v>
       </c>
@@ -4322,7 +4331,7 @@
       <c r="AD23" s="33"/>
       <c r="AE23" s="33"/>
     </row>
-    <row r="24" spans="1:31" s="6" customFormat="1" ht="15" thickBot="1">
+    <row r="24" spans="1:31" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="10"/>
       <c r="B24" s="23" t="s">
         <v>123</v>
@@ -4393,7 +4402,7 @@
       <c r="AD24" s="33"/>
       <c r="AE24" s="33"/>
     </row>
-    <row r="25" spans="1:31">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B25" s="23" t="s">
         <v>124</v>
       </c>
@@ -4448,7 +4457,7 @@
       <c r="AD25" s="33"/>
       <c r="AE25" s="33"/>
     </row>
-    <row r="26" spans="1:31">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B26" s="23" t="s">
         <v>125</v>
       </c>
@@ -4478,7 +4487,7 @@
       <c r="T26" s="83">
         <v>0.5</v>
       </c>
-      <c r="V26" s="75">
+      <c r="V26" s="89">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
@@ -4503,7 +4512,7 @@
       <c r="AD26" s="33"/>
       <c r="AE26" s="33"/>
     </row>
-    <row r="27" spans="1:31">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A27" s="11" t="s">
         <v>77</v>
       </c>
@@ -4575,7 +4584,7 @@
       <c r="AD27" s="33"/>
       <c r="AE27" s="33"/>
     </row>
-    <row r="28" spans="1:31" s="33" customFormat="1">
+    <row r="28" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="10"/>
       <c r="B28" s="23" t="s">
         <v>127</v>
@@ -4658,7 +4667,7 @@
         <v>24.830000000000002</v>
       </c>
     </row>
-    <row r="29" spans="1:31">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B29" s="23" t="s">
         <v>189</v>
       </c>
@@ -4731,7 +4740,7 @@
       <c r="AD29" s="33"/>
       <c r="AE29" s="33"/>
     </row>
-    <row r="30" spans="1:31">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B30" s="23" t="s">
         <v>190</v>
       </c>
@@ -4814,7 +4823,7 @@
         <v>17.680000000000003</v>
       </c>
     </row>
-    <row r="31" spans="1:31">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B31" s="23" t="s">
         <v>128</v>
       </c>
@@ -4878,7 +4887,7 @@
       <c r="AD31" s="33"/>
       <c r="AE31" s="33"/>
     </row>
-    <row r="32" spans="1:31">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B32" s="23" t="s">
         <v>97</v>
       </c>
@@ -4949,7 +4958,7 @@
         <v>11.959999999999999</v>
       </c>
     </row>
-    <row r="33" spans="1:31" s="6" customFormat="1">
+    <row r="33" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="10"/>
       <c r="B33" s="23" t="s">
         <v>98</v>
@@ -5025,7 +5034,7 @@
       <c r="AD33"/>
       <c r="AE33"/>
     </row>
-    <row r="34" spans="1:31" ht="15" thickBot="1">
+    <row r="34" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B34" s="23" t="s">
         <v>95</v>
       </c>
@@ -5090,7 +5099,7 @@
         <v>6.11</v>
       </c>
     </row>
-    <row r="35" spans="1:31" s="33" customFormat="1">
+    <row r="35" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="10"/>
       <c r="B35" s="23" t="s">
         <v>129</v>
@@ -5151,7 +5160,7 @@
       <c r="U35" s="83">
         <v>1</v>
       </c>
-      <c r="V35" s="75">
+      <c r="V35" s="89">
         <f t="shared" si="1"/>
         <v>3.25</v>
       </c>
@@ -5164,7 +5173,7 @@
       <c r="AD35"/>
       <c r="AE35"/>
     </row>
-    <row r="36" spans="1:31">
+    <row r="36" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A36" s="11" t="s">
         <v>78</v>
       </c>
@@ -5239,7 +5248,7 @@
       <c r="AD36" s="6"/>
       <c r="AE36" s="6"/>
     </row>
-    <row r="37" spans="1:31">
+    <row r="37" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B37" s="23" t="s">
         <v>174</v>
       </c>
@@ -5305,7 +5314,7 @@
       <c r="Z37" s="33"/>
       <c r="AA37" s="33"/>
     </row>
-    <row r="38" spans="1:31">
+    <row r="38" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B38" s="23" t="s">
         <v>192</v>
       </c>
@@ -5340,7 +5349,7 @@
       <c r="AD38" s="33"/>
       <c r="AE38" s="33"/>
     </row>
-    <row r="39" spans="1:31">
+    <row r="39" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B39" s="23" t="s">
         <v>131</v>
       </c>
@@ -5398,7 +5407,7 @@
       <c r="W39" s="33"/>
       <c r="X39" s="80"/>
     </row>
-    <row r="40" spans="1:31">
+    <row r="40" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B40" s="23" t="s">
         <v>217</v>
       </c>
@@ -5451,14 +5460,14 @@
       <c r="T40" s="83">
         <v>1</v>
       </c>
-      <c r="V40" s="75">
+      <c r="V40" s="89">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="W40" s="33"/>
       <c r="X40" s="80"/>
     </row>
-    <row r="41" spans="1:31">
+    <row r="41" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A41" s="11" t="s">
         <v>79</v>
       </c>
@@ -5531,7 +5540,7 @@
       <c r="X41" s="80"/>
       <c r="AA41" s="6"/>
     </row>
-    <row r="42" spans="1:31" s="6" customFormat="1">
+    <row r="42" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="10"/>
       <c r="B42" s="23" t="s">
         <v>93</v>
@@ -5608,7 +5617,7 @@
       <c r="AD42"/>
       <c r="AE42"/>
     </row>
-    <row r="43" spans="1:31">
+    <row r="43" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B43" s="23" t="s">
         <v>132</v>
       </c>
@@ -5673,7 +5682,7 @@
       <c r="X43" s="15"/>
       <c r="Y43" s="6"/>
     </row>
-    <row r="44" spans="1:31">
+    <row r="44" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B44" s="23" t="s">
         <v>216</v>
       </c>
@@ -5716,14 +5725,14 @@
       <c r="T44" s="83">
         <v>0.75</v>
       </c>
-      <c r="V44" s="75">
+      <c r="V44" s="89">
         <f t="shared" si="1"/>
         <v>0.75</v>
       </c>
       <c r="W44" s="33"/>
       <c r="AA44" s="6"/>
     </row>
-    <row r="45" spans="1:31">
+    <row r="45" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A45" s="11" t="s">
         <v>80</v>
       </c>
@@ -5782,7 +5791,7 @@
       </c>
       <c r="W45" s="33"/>
     </row>
-    <row r="46" spans="1:31">
+    <row r="46" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B46" s="23" t="s">
         <v>133</v>
       </c>
@@ -5829,7 +5838,7 @@
       <c r="U46" s="83">
         <v>1</v>
       </c>
-      <c r="V46" s="75">
+      <c r="V46" s="89">
         <f t="shared" si="1"/>
         <v>2.75</v>
       </c>
@@ -5840,7 +5849,7 @@
       <c r="AD46" s="6"/>
       <c r="AE46" s="6"/>
     </row>
-    <row r="47" spans="1:31" s="6" customFormat="1">
+    <row r="47" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="11" t="s">
         <v>81</v>
       </c>
@@ -5908,7 +5917,7 @@
       <c r="AD47"/>
       <c r="AE47"/>
     </row>
-    <row r="48" spans="1:31">
+    <row r="48" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B48" s="23" t="s">
         <v>135</v>
       </c>
@@ -5972,7 +5981,7 @@
       <c r="W48" s="33"/>
       <c r="Z48" s="6"/>
     </row>
-    <row r="49" spans="1:31">
+    <row r="49" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B49" s="23" t="s">
         <v>136</v>
       </c>
@@ -6026,7 +6035,7 @@
       </c>
       <c r="W49" s="33"/>
     </row>
-    <row r="50" spans="1:31" s="6" customFormat="1">
+    <row r="50" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="10"/>
       <c r="B50" s="23" t="s">
         <v>137</v>
@@ -6085,7 +6094,7 @@
       <c r="AD50"/>
       <c r="AE50"/>
     </row>
-    <row r="51" spans="1:31">
+    <row r="51" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B51" s="23" t="s">
         <v>138</v>
       </c>
@@ -6148,7 +6157,7 @@
       </c>
       <c r="W51" s="33"/>
     </row>
-    <row r="52" spans="1:31" s="6" customFormat="1">
+    <row r="52" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="10"/>
       <c r="B52" s="23" t="s">
         <v>139</v>
@@ -6217,7 +6226,7 @@
       <c r="AD52"/>
       <c r="AE52"/>
     </row>
-    <row r="53" spans="1:31">
+    <row r="53" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B53" s="23" t="s">
         <v>140</v>
       </c>
@@ -6277,7 +6286,7 @@
       </c>
       <c r="W53" s="33"/>
     </row>
-    <row r="54" spans="1:31">
+    <row r="54" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B54" s="23" t="s">
         <v>141</v>
       </c>
@@ -6343,7 +6352,7 @@
       <c r="AD54" s="6"/>
       <c r="AE54" s="6"/>
     </row>
-    <row r="55" spans="1:31">
+    <row r="55" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B55" s="23" t="s">
         <v>96</v>
       </c>
@@ -6389,7 +6398,7 @@
       <c r="W55" s="33"/>
       <c r="AB55" s="33"/>
     </row>
-    <row r="56" spans="1:31">
+    <row r="56" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B56" s="23" t="s">
         <v>142</v>
       </c>
@@ -6437,7 +6446,7 @@
       <c r="W56" s="33"/>
       <c r="AB56" s="33"/>
     </row>
-    <row r="57" spans="1:31">
+    <row r="57" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B57" s="23" t="s">
         <v>143</v>
       </c>
@@ -6477,7 +6486,7 @@
       <c r="Z57" s="6"/>
       <c r="AB57" s="33"/>
     </row>
-    <row r="58" spans="1:31">
+    <row r="58" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B58" s="23" t="s">
         <v>144</v>
       </c>
@@ -6519,7 +6528,7 @@
       <c r="W58" s="33"/>
       <c r="AB58" s="33"/>
     </row>
-    <row r="59" spans="1:31">
+    <row r="59" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B59" s="23" t="s">
         <v>145</v>
       </c>
@@ -6558,7 +6567,7 @@
       <c r="T59" s="83">
         <v>0.5</v>
       </c>
-      <c r="V59" s="75">
+      <c r="V59" s="89">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
@@ -6566,7 +6575,7 @@
       <c r="AA59" s="6"/>
       <c r="AB59" s="33"/>
     </row>
-    <row r="60" spans="1:31">
+    <row r="60" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A60" s="11" t="s">
         <v>82</v>
       </c>
@@ -6626,7 +6635,7 @@
       <c r="W60" s="33"/>
       <c r="AB60" s="33"/>
     </row>
-    <row r="61" spans="1:31">
+    <row r="61" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B61" s="23" t="s">
         <v>147</v>
       </c>
@@ -6662,7 +6671,7 @@
       <c r="W61" s="33"/>
       <c r="AB61" s="33"/>
     </row>
-    <row r="62" spans="1:31">
+    <row r="62" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B62" s="23" t="s">
         <v>148</v>
       </c>
@@ -6698,7 +6707,7 @@
       <c r="AD62" s="6"/>
       <c r="AE62" s="6"/>
     </row>
-    <row r="63" spans="1:31">
+    <row r="63" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A63" s="48"/>
       <c r="B63" s="24" t="s">
         <v>149</v>
@@ -6737,7 +6746,7 @@
       </c>
       <c r="T63" s="86"/>
       <c r="U63" s="86"/>
-      <c r="V63" s="75">
+      <c r="V63" s="89">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -6745,7 +6754,7 @@
       <c r="AA63" s="6"/>
       <c r="AB63" s="33"/>
     </row>
-    <row r="64" spans="1:31">
+    <row r="64" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A64" s="10" t="s">
         <v>83</v>
       </c>
@@ -6783,7 +6792,7 @@
       <c r="W64" s="33"/>
       <c r="AB64" s="33"/>
     </row>
-    <row r="65" spans="1:31" s="6" customFormat="1">
+    <row r="65" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="10"/>
       <c r="B65" s="23" t="s">
         <v>151</v>
@@ -6834,7 +6843,7 @@
       <c r="AD65"/>
       <c r="AE65"/>
     </row>
-    <row r="66" spans="1:31">
+    <row r="66" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B66" s="23" t="s">
         <v>205</v>
       </c>
@@ -6861,13 +6870,13 @@
       <c r="P66" s="83">
         <v>1</v>
       </c>
-      <c r="V66" s="75">
+      <c r="V66" s="89">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="W66" s="33"/>
     </row>
-    <row r="67" spans="1:31">
+    <row r="67" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A67" s="11" t="s">
         <v>84</v>
       </c>
@@ -6922,7 +6931,7 @@
       </c>
       <c r="W67" s="33"/>
     </row>
-    <row r="68" spans="1:31">
+    <row r="68" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A68" s="30"/>
       <c r="B68" s="31" t="s">
         <v>99</v>
@@ -6968,7 +6977,7 @@
       <c r="Y68" s="33"/>
       <c r="AA68" s="6"/>
     </row>
-    <row r="69" spans="1:31" s="6" customFormat="1">
+    <row r="69" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A69" s="10"/>
       <c r="B69" s="23" t="s">
         <v>153</v>
@@ -7031,7 +7040,7 @@
       <c r="AD69"/>
       <c r="AE69"/>
     </row>
-    <row r="70" spans="1:31">
+    <row r="70" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B70" s="23" t="s">
         <v>154</v>
       </c>
@@ -7079,7 +7088,7 @@
       <c r="AD70" s="6"/>
       <c r="AE70" s="6"/>
     </row>
-    <row r="71" spans="1:31" s="33" customFormat="1">
+    <row r="71" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A71" s="10"/>
       <c r="B71" s="23" t="s">
         <v>155</v>
@@ -7116,7 +7125,7 @@
       <c r="AD71"/>
       <c r="AE71"/>
     </row>
-    <row r="72" spans="1:31">
+    <row r="72" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B72" s="23" t="s">
         <v>156</v>
       </c>
@@ -7145,7 +7154,7 @@
       </c>
       <c r="W72" s="33"/>
     </row>
-    <row r="73" spans="1:31">
+    <row r="73" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B73" s="23" t="s">
         <v>157</v>
       </c>
@@ -7179,7 +7188,7 @@
       <c r="Z73" s="33"/>
       <c r="AA73" s="33"/>
     </row>
-    <row r="74" spans="1:31" s="6" customFormat="1">
+    <row r="74" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A74" s="10"/>
       <c r="B74" s="24" t="s">
         <v>202</v>
@@ -7224,7 +7233,7 @@
         <v>1</v>
       </c>
       <c r="U74" s="86"/>
-      <c r="V74" s="75">
+      <c r="V74" s="89">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
@@ -7238,11 +7247,11 @@
       <c r="AD74" s="33"/>
       <c r="AE74" s="33"/>
     </row>
-    <row r="75" spans="1:31" ht="15" thickBot="1">
+    <row r="75" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A75" s="11"/>
       <c r="W75" s="15"/>
     </row>
-    <row r="76" spans="1:31">
+    <row r="76" spans="1:31" x14ac:dyDescent="0.3">
       <c r="K76" s="64" t="s">
         <v>165</v>
       </c>
@@ -7280,7 +7289,7 @@
       <c r="AD76" s="6"/>
       <c r="AE76" s="6"/>
     </row>
-    <row r="77" spans="1:31">
+    <row r="77" spans="1:31" x14ac:dyDescent="0.3">
       <c r="K77" s="67" t="s">
         <v>167</v>
       </c>
@@ -7314,7 +7323,7 @@
       <c r="U77" s="68"/>
       <c r="W77" s="15"/>
     </row>
-    <row r="78" spans="1:31" s="33" customFormat="1">
+    <row r="78" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A78" s="10"/>
       <c r="B78" s="23"/>
       <c r="C78" s="23"/>
@@ -7367,7 +7376,7 @@
       <c r="AD78" s="6"/>
       <c r="AE78" s="6"/>
     </row>
-    <row r="79" spans="1:31">
+    <row r="79" spans="1:31" x14ac:dyDescent="0.3">
       <c r="K79" s="67" t="s">
         <v>168</v>
       </c>
@@ -7400,7 +7409,7 @@
       <c r="T79" s="68"/>
       <c r="U79" s="68"/>
     </row>
-    <row r="80" spans="1:31">
+    <row r="80" spans="1:31" x14ac:dyDescent="0.3">
       <c r="K80" s="67" t="s">
         <v>169</v>
       </c>
@@ -7440,7 +7449,7 @@
       <c r="AD80" s="6"/>
       <c r="AE80" s="6"/>
     </row>
-    <row r="81" spans="1:31" ht="15" thickBot="1">
+    <row r="81" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D81" s="33"/>
       <c r="K81" s="72" t="s">
         <v>90</v>
@@ -7478,19 +7487,19 @@
       <c r="AD81" s="6"/>
       <c r="AE81" s="6"/>
     </row>
-    <row r="82" spans="1:31">
+    <row r="82" spans="1:31" x14ac:dyDescent="0.3">
       <c r="D82" s="33"/>
     </row>
-    <row r="83" spans="1:31">
+    <row r="83" spans="1:31" x14ac:dyDescent="0.3">
       <c r="D83" s="33"/>
     </row>
-    <row r="84" spans="1:31">
+    <row r="84" spans="1:31" x14ac:dyDescent="0.3">
       <c r="D84" s="33"/>
     </row>
-    <row r="85" spans="1:31">
+    <row r="85" spans="1:31" x14ac:dyDescent="0.3">
       <c r="AA85" s="33"/>
     </row>
-    <row r="88" spans="1:31" s="33" customFormat="1">
+    <row r="88" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A88" s="10"/>
       <c r="B88" s="23"/>
       <c r="C88" s="23"/>
@@ -7523,25 +7532,25 @@
       <c r="AD88"/>
       <c r="AE88"/>
     </row>
-    <row r="94" spans="1:31">
+    <row r="94" spans="1:31" x14ac:dyDescent="0.3">
       <c r="AB94" s="6"/>
       <c r="AC94" s="6"/>
       <c r="AD94" s="6"/>
       <c r="AE94" s="6"/>
     </row>
-    <row r="98" spans="28:31">
+    <row r="98" spans="28:31" x14ac:dyDescent="0.3">
       <c r="AB98" s="6"/>
       <c r="AC98" s="6"/>
       <c r="AD98" s="6"/>
       <c r="AE98" s="6"/>
     </row>
-    <row r="103" spans="28:31">
+    <row r="103" spans="28:31" x14ac:dyDescent="0.3">
       <c r="AB103" s="6"/>
       <c r="AC103" s="6"/>
       <c r="AD103" s="6"/>
       <c r="AE103" s="6"/>
     </row>
-    <row r="116" spans="28:31">
+    <row r="116" spans="28:31" x14ac:dyDescent="0.3">
       <c r="AB116" s="33"/>
       <c r="AC116" s="33"/>
       <c r="AD116" s="33"/>
@@ -7600,372 +7609,372 @@
       <selection sqref="A1:A73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="50.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="50.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:1">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:1">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:1">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:1">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:1">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:1">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:1">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:1">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:1">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:1">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:1">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:1">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:1">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:1">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:1">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:1">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:1">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:1">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:1">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:1">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:1">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="69" spans="1:1">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:1">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:1">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:1">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:1">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>71</v>
       </c>

</xml_diff>